<commit_message>
Analyzer - Add failure check feature in data diagnosis (#378)
**Description**
Add failure check feature in data diagnosis.

**Major Revision**
- Add failure check rule op to support that if there exists metric_regex not been matched by any metric in result, label as failedtest
- Split performance issue and failedtest in categories


**Minor Revision**
- replace DataFrame.append() with pd.concat since append() will be removed in later version of pandas
</commit_message>
<xml_diff>
--- a/tests/data/diagnosis_summary.xlsx
+++ b/tests/data/diagnosis_summary.xlsx
@@ -1421,7 +1421,7 @@
     <t>KernelLaunch</t>
   </si>
   <si>
-    <t>FailedTest,Mem</t>
+    <t>FailedTest</t>
   </si>
   <si>
     <t>kernel-launch/event_overhead:0(B/L: 0.0060 VAL: 0.1000 VAR: 1577.85% Rule:lambda x:x&gt;0.05)</t>
@@ -7597,88 +7597,88 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AA2:AA3">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="47">
+      <formula>LEN(TRIM(AA2))&gt;0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="48" operator="lessThan">
+      <formula>-0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB2:AB3">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="37">
+      <formula>LEN(TRIM(AB2))&gt;0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="38" operator="lessThan">
+      <formula>-0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC2:AC3">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="63">
+      <formula>LEN(TRIM(AC2))&gt;0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="64" operator="lessThan">
+      <formula>-0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD2:AD3">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="41">
+      <formula>LEN(TRIM(AD2))&gt;0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="42" operator="lessThan">
+      <formula>-0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE2:AE3">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="59">
+      <formula>LEN(TRIM(AE2))&gt;0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="60" operator="lessThan">
+      <formula>-0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF2:AF3">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="51">
+      <formula>LEN(TRIM(AF2))&gt;0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="52" operator="lessThan">
+      <formula>-0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG2:AG3">
     <cfRule type="notContainsBlanks" dxfId="0" priority="39">
-      <formula>LEN(TRIM(AA2))&gt;0</formula>
+      <formula>LEN(TRIM(AG2))&gt;0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="40" operator="lessThan">
       <formula>-0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB2:AB3">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="55">
-      <formula>LEN(TRIM(AB2))&gt;0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="56" operator="lessThan">
-      <formula>-0.05</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC2:AC3">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="43">
-      <formula>LEN(TRIM(AC2))&gt;0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="44" operator="lessThan">
-      <formula>-0.05</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD2:AD3">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="61">
-      <formula>LEN(TRIM(AD2))&gt;0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="62" operator="lessThan">
-      <formula>-0.05</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE2:AE3">
+  <conditionalFormatting sqref="AH2:AH3">
     <cfRule type="notContainsBlanks" dxfId="0" priority="35">
-      <formula>LEN(TRIM(AE2))&gt;0</formula>
+      <formula>LEN(TRIM(AH2))&gt;0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="36" operator="lessThan">
       <formula>-0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF2:AF3">
+  <conditionalFormatting sqref="AI2:AI3">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="57">
+      <formula>LEN(TRIM(AI2))&gt;0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="58" operator="lessThan">
+      <formula>-0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ2:AJ3">
     <cfRule type="notContainsBlanks" dxfId="0" priority="45">
-      <formula>LEN(TRIM(AF2))&gt;0</formula>
+      <formula>LEN(TRIM(AJ2))&gt;0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="46" operator="lessThan">
       <formula>-0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG2:AG3">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="57">
-      <formula>LEN(TRIM(AG2))&gt;0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="58" operator="lessThan">
-      <formula>-0.05</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH2:AH3">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="63">
-      <formula>LEN(TRIM(AH2))&gt;0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="64" operator="lessThan">
-      <formula>-0.05</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AI2:AI3">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="37">
-      <formula>LEN(TRIM(AI2))&gt;0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="38" operator="lessThan">
-      <formula>-0.05</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ2:AJ3">
+  <conditionalFormatting sqref="AK2:AK3">
     <cfRule type="cellIs" dxfId="1" priority="66" operator="greaterThan">
       <formula>0.0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C3">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="19">
-      <formula>LEN(TRIM(C2))&gt;0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="20" operator="greaterThan">
-      <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D3">
@@ -7690,95 +7690,95 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E3">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="21">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(E2))&gt;0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F3">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="31">
+      <formula>LEN(TRIM(F2))&gt;0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="32" operator="greaterThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G3">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="11">
+      <formula>LEN(TRIM(G2))&gt;0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="12" operator="greaterThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H3">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="29">
+      <formula>LEN(TRIM(H2))&gt;0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="30" operator="greaterThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I3">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="3">
+      <formula>LEN(TRIM(I2))&gt;0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J3">
     <cfRule type="notContainsBlanks" dxfId="0" priority="15">
-      <formula>LEN(TRIM(F2))&gt;0</formula>
+      <formula>LEN(TRIM(J2))&gt;0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="16" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="13">
-      <formula>LEN(TRIM(G2))&gt;0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="14" operator="greaterThan">
-      <formula>0.05</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="3">
-      <formula>LEN(TRIM(H2))&gt;0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThan">
-      <formula>0.05</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I3">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="27">
-      <formula>LEN(TRIM(I2))&gt;0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="28" operator="greaterThan">
-      <formula>0.05</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J3">
+  <conditionalFormatting sqref="K2:K3">
     <cfRule type="notContainsBlanks" dxfId="0" priority="5">
-      <formula>LEN(TRIM(J2))&gt;0</formula>
+      <formula>LEN(TRIM(K2))&gt;0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="6" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K3">
+  <conditionalFormatting sqref="L2:L3">
     <cfRule type="cellIs" dxfId="1" priority="65" operator="greaterThan">
       <formula>0.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L3">
+  <conditionalFormatting sqref="M2:M3">
     <cfRule type="notContainsBlanks" dxfId="0" priority="17">
-      <formula>LEN(TRIM(L2))&gt;0</formula>
+      <formula>LEN(TRIM(M2))&gt;0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="18" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M3">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="31">
-      <formula>LEN(TRIM(M2))&gt;0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="32" operator="greaterThan">
-      <formula>0.05</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="N2:N3">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="23">
       <formula>LEN(TRIM(N2))&gt;0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="24" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O3">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="7">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="19">
       <formula>LEN(TRIM(O2))&gt;0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="20" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P3">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="23">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="7">
       <formula>LEN(TRIM(P2))&gt;0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7791,74 +7791,74 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R3">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="29">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="27">
       <formula>LEN(TRIM(R2))&gt;0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="28" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S3">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="11">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="13">
       <formula>LEN(TRIM(S2))&gt;0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="14" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T3">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="21">
+      <formula>LEN(TRIM(T2))&gt;0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="22" operator="greaterThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U2:U3">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="49">
+      <formula>LEN(TRIM(U2))&gt;0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="50" operator="lessThan">
+      <formula>-0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V2:V3">
     <cfRule type="notContainsBlanks" dxfId="0" priority="33">
-      <formula>LEN(TRIM(T2))&gt;0</formula>
+      <formula>LEN(TRIM(V2))&gt;0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="34" operator="lessThan">
       <formula>-0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U2:U3">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="47">
-      <formula>LEN(TRIM(U2))&gt;0</formula>
+  <conditionalFormatting sqref="W2:W3">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="61">
+      <formula>LEN(TRIM(W2))&gt;0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="48" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="62" operator="lessThan">
       <formula>-0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V2:V3">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="51">
-      <formula>LEN(TRIM(V2))&gt;0</formula>
+  <conditionalFormatting sqref="X2:X3">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="55">
+      <formula>LEN(TRIM(X2))&gt;0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="52" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="56" operator="lessThan">
       <formula>-0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W2:W3">
+  <conditionalFormatting sqref="Y2:Y3">
     <cfRule type="notContainsBlanks" dxfId="0" priority="53">
-      <formula>LEN(TRIM(W2))&gt;0</formula>
+      <formula>LEN(TRIM(Y2))&gt;0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="54" operator="lessThan">
       <formula>-0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X2:X3">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="49">
-      <formula>LEN(TRIM(X2))&gt;0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="50" operator="lessThan">
-      <formula>-0.05</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y2:Y3">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="59">
-      <formula>LEN(TRIM(Y2))&gt;0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="60" operator="lessThan">
-      <formula>-0.05</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="Z2:Z3">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="41">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="43">
       <formula>LEN(TRIM(Z2))&gt;0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="42" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="44" operator="lessThan">
       <formula>-0.05</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>